<commit_message>
da finire la visualizzazione della data e delle ore con l'orologio che ticchetta
</commit_message>
<xml_diff>
--- a/windows_form_app/bin/Debug/ConditionalFormatColorScale.xlsx
+++ b/windows_form_app/bin/Debug/ConditionalFormatColorScale.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="Rac0b9d6da0d84ead"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R7752bb3ad6dc46bf"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -345,642 +345,642 @@
   <x:sheetData>
     <x:row r="1">
       <x:c r="A1">
-        <x:v>132.345860699353</x:v>
+        <x:v>148.229717625412</x:v>
       </x:c>
       <x:c r="B1">
-        <x:v>19.727031616367</x:v>
+        <x:v>111.604122310693</x:v>
       </x:c>
       <x:c r="C1">
-        <x:v>57.0660177883999</x:v>
+        <x:v>13.2234045365934</x:v>
       </x:c>
       <x:c r="D1">
-        <x:v>104.275475118438</x:v>
+        <x:v>32.5750158320065</x:v>
       </x:c>
       <x:c r="E1">
-        <x:v>162.760762014781</x:v>
+        <x:v>118.067045751059</x:v>
       </x:c>
       <x:c r="F1">
-        <x:v>76.3545577769887</x:v>
+        <x:v>157.447280063036</x:v>
       </x:c>
       <x:c r="G1">
-        <x:v>134.015239930719</x:v>
+        <x:v>182.540780763394</x:v>
       </x:c>
       <x:c r="H1">
-        <x:v>61.7426252280095</x:v>
+        <x:v>80.4811589794611</x:v>
       </x:c>
       <x:c r="I1">
-        <x:v>181.288647642959</x:v>
+        <x:v>172.439766289871</x:v>
       </x:c>
       <x:c r="J1">
-        <x:v>108.586283544351</x:v>
+        <x:v>165.571800044538</x:v>
       </x:c>
     </x:row>
     <x:row r="2">
       <x:c r="A2">
-        <x:v>197.2855696442</x:v>
+        <x:v>112.433960154855</x:v>
       </x:c>
       <x:c r="B2">
-        <x:v>22.5190807238776</x:v>
+        <x:v>103.396801139878</x:v>
       </x:c>
       <x:c r="C2">
-        <x:v>101.499123732326</x:v>
+        <x:v>141.047907779481</x:v>
       </x:c>
       <x:c r="D2">
-        <x:v>132.508528014882</x:v>
+        <x:v>98.9095377265054</x:v>
       </x:c>
       <x:c r="E2">
-        <x:v>121.886156276747</x:v>
+        <x:v>163.981578016645</x:v>
       </x:c>
       <x:c r="F2">
-        <x:v>4.75364560482728</x:v>
+        <x:v>100.985078094986</x:v>
       </x:c>
       <x:c r="G2">
-        <x:v>102.035285021195</x:v>
+        <x:v>56.6176130700007</x:v>
       </x:c>
       <x:c r="H2">
-        <x:v>31.8399254380911</x:v>
+        <x:v>64.1690493860138</x:v>
       </x:c>
       <x:c r="I2">
-        <x:v>187.396332336309</x:v>
+        <x:v>128.105025704999</x:v>
       </x:c>
       <x:c r="J2">
-        <x:v>172.694830863129</x:v>
+        <x:v>31.6074366828461</x:v>
       </x:c>
     </x:row>
     <x:row r="3">
       <x:c r="A3">
-        <x:v>102.947662632422</x:v>
+        <x:v>198.738175257453</x:v>
       </x:c>
       <x:c r="B3">
-        <x:v>159.634085725823</x:v>
+        <x:v>153.875191488245</x:v>
       </x:c>
       <x:c r="C3">
-        <x:v>44.9718804308082</x:v>
+        <x:v>199.13598578383</x:v>
       </x:c>
       <x:c r="D3">
-        <x:v>74.9730997136669</x:v>
+        <x:v>193.675257542019</x:v>
       </x:c>
       <x:c r="E3">
-        <x:v>172.107331255501</x:v>
+        <x:v>164.058820234639</x:v>
       </x:c>
       <x:c r="F3">
-        <x:v>45.4228528986791</x:v>
+        <x:v>163.385138829884</x:v>
       </x:c>
       <x:c r="G3">
-        <x:v>25.3892616487058</x:v>
+        <x:v>100.500519527355</x:v>
       </x:c>
       <x:c r="H3">
-        <x:v>111.461722809571</x:v>
+        <x:v>120.475367047114</x:v>
       </x:c>
       <x:c r="I3">
-        <x:v>194.178133082659</x:v>
+        <x:v>171.336902292137</x:v>
       </x:c>
       <x:c r="J3">
-        <x:v>63.653266459542</x:v>
+        <x:v>91.3067922421297</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
       <x:c r="A4">
-        <x:v>183.977587793012</x:v>
+        <x:v>6.58374904030177</x:v>
       </x:c>
       <x:c r="B4">
-        <x:v>154.006525759588</x:v>
+        <x:v>58.4566431392248</x:v>
       </x:c>
       <x:c r="C4">
-        <x:v>45.8412296352169</x:v>
+        <x:v>95.5408974995561</x:v>
       </x:c>
       <x:c r="D4">
-        <x:v>145.661894486128</x:v>
+        <x:v>67.6215193549271</x:v>
       </x:c>
       <x:c r="E4">
-        <x:v>89.0358835873361</x:v>
+        <x:v>13.1260387660591</x:v>
       </x:c>
       <x:c r="F4">
-        <x:v>144.437983233686</x:v>
+        <x:v>122.829748840458</x:v>
       </x:c>
       <x:c r="G4">
-        <x:v>153.054654203846</x:v>
+        <x:v>71.961750123632</x:v>
       </x:c>
       <x:c r="H4">
-        <x:v>180.602385001538</x:v>
+        <x:v>172.44797384946</x:v>
       </x:c>
       <x:c r="I4">
-        <x:v>92.6974176860868</x:v>
+        <x:v>73.8501658075723</x:v>
       </x:c>
       <x:c r="J4">
-        <x:v>190.862882971234</x:v>
+        <x:v>133.056453118593</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
       <x:c r="A5">
-        <x:v>142.791561941985</x:v>
+        <x:v>129.587843143189</x:v>
       </x:c>
       <x:c r="B5">
-        <x:v>192.679715153146</x:v>
+        <x:v>95.1301574218693</x:v>
       </x:c>
       <x:c r="C5">
-        <x:v>76.6083867645862</x:v>
+        <x:v>162.057416589026</x:v>
       </x:c>
       <x:c r="D5">
-        <x:v>188.744419249121</x:v>
+        <x:v>139.110995800752</x:v>
       </x:c>
       <x:c r="E5">
-        <x:v>186.117463924977</x:v>
+        <x:v>1.66322710069978</x:v>
       </x:c>
       <x:c r="F5">
-        <x:v>111.384872585249</x:v>
+        <x:v>5.37442770105527</x:v>
       </x:c>
       <x:c r="G5">
-        <x:v>101.266214112409</x:v>
+        <x:v>112.940371275386</x:v>
       </x:c>
       <x:c r="H5">
-        <x:v>86.1486544302426</x:v>
+        <x:v>140.08451920938</x:v>
       </x:c>
       <x:c r="I5">
-        <x:v>80.4410351814893</x:v>
+        <x:v>106.081263025329</x:v>
       </x:c>
       <x:c r="J5">
-        <x:v>6.75439779029898</x:v>
+        <x:v>198.192902281039</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
       <x:c r="A6">
-        <x:v>122.626623475285</x:v>
+        <x:v>149.330897791931</x:v>
       </x:c>
       <x:c r="B6">
-        <x:v>83.3278273620307</x:v>
+        <x:v>76.3430363854128</x:v>
       </x:c>
       <x:c r="C6">
-        <x:v>176.740418829369</x:v>
+        <x:v>145.286550347361</x:v>
       </x:c>
       <x:c r="D6">
-        <x:v>70.3407942644976</x:v>
+        <x:v>140.395605256965</x:v>
       </x:c>
       <x:c r="E6">
-        <x:v>176.557949453852</x:v>
+        <x:v>179.028062233249</x:v>
       </x:c>
       <x:c r="F6">
-        <x:v>172.71177497353</x:v>
+        <x:v>194.354526137167</x:v>
       </x:c>
       <x:c r="G6">
-        <x:v>174.755151185559</x:v>
+        <x:v>112.468136526862</x:v>
       </x:c>
       <x:c r="H6">
-        <x:v>182.092918074733</x:v>
+        <x:v>19.5481469945741</x:v>
       </x:c>
       <x:c r="I6">
-        <x:v>132.168143862937</x:v>
+        <x:v>68.5161955973675</x:v>
       </x:c>
       <x:c r="J6">
-        <x:v>117.337909116101</x:v>
+        <x:v>154.681906921175</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
       <x:c r="A7">
-        <x:v>50.9652961282829</x:v>
+        <x:v>56.946760535681</x:v>
       </x:c>
       <x:c r="B7">
-        <x:v>22.5535171211481</x:v>
+        <x:v>62.0654137162796</x:v>
       </x:c>
       <x:c r="C7">
-        <x:v>67.5644921453504</x:v>
+        <x:v>109.144256687325</x:v>
       </x:c>
       <x:c r="D7">
-        <x:v>117.635381183417</x:v>
+        <x:v>81.1329740477414</x:v>
       </x:c>
       <x:c r="E7">
-        <x:v>124.60869575134</x:v>
+        <x:v>158.988051004237</x:v>
       </x:c>
       <x:c r="F7">
-        <x:v>43.2790438846122</x:v>
+        <x:v>53.9773170156299</x:v>
       </x:c>
       <x:c r="G7">
-        <x:v>176.677851088661</x:v>
+        <x:v>7.85590364032234</x:v>
       </x:c>
       <x:c r="H7">
-        <x:v>155.837229246198</x:v>
+        <x:v>73.4263884245541</x:v>
       </x:c>
       <x:c r="I7">
-        <x:v>43.4726444275457</x:v>
+        <x:v>85.7834989604463</x:v>
       </x:c>
       <x:c r="J7">
-        <x:v>177.448173043061</x:v>
+        <x:v>41.1518291761874</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
       <x:c r="A8">
-        <x:v>51.6989914009809</x:v>
+        <x:v>29.0233279713538</x:v>
       </x:c>
       <x:c r="B8">
-        <x:v>121.432900019657</x:v>
+        <x:v>84.1696392205402</x:v>
       </x:c>
       <x:c r="C8">
-        <x:v>139.142507752004</x:v>
+        <x:v>190.318883578442</x:v>
       </x:c>
       <x:c r="D8">
-        <x:v>196.533449365074</x:v>
+        <x:v>195.048572586406</x:v>
       </x:c>
       <x:c r="E8">
-        <x:v>29.903268921144</x:v>
+        <x:v>102.019593539657</x:v>
       </x:c>
       <x:c r="F8">
-        <x:v>110.267947479276</x:v>
+        <x:v>103.608017835584</x:v>
       </x:c>
       <x:c r="G8">
-        <x:v>83.0256989612364</x:v>
+        <x:v>191.817774899219</x:v>
       </x:c>
       <x:c r="H8">
-        <x:v>56.2274611816869</x:v>
+        <x:v>60.0249899830786</x:v>
       </x:c>
       <x:c r="I8">
-        <x:v>88.8556357886901</x:v>
+        <x:v>192.01203044132</x:v>
       </x:c>
       <x:c r="J8">
-        <x:v>60.7224586702522</x:v>
+        <x:v>158.684392533584</x:v>
       </x:c>
     </x:row>
     <x:row r="9">
       <x:c r="A9">
-        <x:v>144.15663878627</x:v>
+        <x:v>50.4447675544977</x:v>
       </x:c>
       <x:c r="B9">
-        <x:v>139.240607218463</x:v>
+        <x:v>160.416000317976</x:v>
       </x:c>
       <x:c r="C9">
-        <x:v>31.0206876280814</x:v>
+        <x:v>14.3941040217849</x:v>
       </x:c>
       <x:c r="D9">
-        <x:v>187.42373529236</x:v>
+        <x:v>173.144000011098</x:v>
       </x:c>
       <x:c r="E9">
-        <x:v>141.026642984257</x:v>
+        <x:v>141.975894450199</x:v>
       </x:c>
       <x:c r="F9">
-        <x:v>100.649760430981</x:v>
+        <x:v>130.240712654889</x:v>
       </x:c>
       <x:c r="G9">
-        <x:v>177.26610693022</x:v>
+        <x:v>113.170092791864</x:v>
       </x:c>
       <x:c r="H9">
-        <x:v>175.500435370719</x:v>
+        <x:v>155.145292242591</x:v>
       </x:c>
       <x:c r="I9">
-        <x:v>169.103945032276</x:v>
+        <x:v>88.5934571216784</x:v>
       </x:c>
       <x:c r="J9">
-        <x:v>116.324108613806</x:v>
+        <x:v>18.7715126288922</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
       <x:c r="A10">
-        <x:v>169.682832048127</x:v>
+        <x:v>10.3616123135954</x:v>
       </x:c>
       <x:c r="B10">
-        <x:v>170.961736129113</x:v>
+        <x:v>52.413603129058</x:v>
       </x:c>
       <x:c r="C10">
-        <x:v>48.4342411386009</x:v>
+        <x:v>103.931778252093</x:v>
       </x:c>
       <x:c r="D10">
-        <x:v>175.359508569985</x:v>
+        <x:v>119.168258886397</x:v>
       </x:c>
       <x:c r="E10">
-        <x:v>139.897586842951</x:v>
+        <x:v>76.1096925829117</x:v>
       </x:c>
       <x:c r="F10">
-        <x:v>120.238044820837</x:v>
+        <x:v>67.5224294269096</x:v>
       </x:c>
       <x:c r="G10">
-        <x:v>125.115223007796</x:v>
+        <x:v>185.985900734545</x:v>
       </x:c>
       <x:c r="H10">
-        <x:v>158.973005581169</x:v>
+        <x:v>80.9244425412847</x:v>
       </x:c>
       <x:c r="I10">
-        <x:v>64.1357234977818</x:v>
+        <x:v>180.122944796515</x:v>
       </x:c>
       <x:c r="J10">
-        <x:v>142.838420040365</x:v>
+        <x:v>147.68591008507</x:v>
       </x:c>
     </x:row>
     <x:row r="11">
       <x:c r="A11">
-        <x:v>134.707021496588</x:v>
+        <x:v>197.518524060733</x:v>
       </x:c>
       <x:c r="B11">
-        <x:v>145.428984866212</x:v>
+        <x:v>39.5139828508319</x:v>
       </x:c>
       <x:c r="C11">
-        <x:v>42.6760100026969</x:v>
+        <x:v>54.3010202489332</x:v>
       </x:c>
       <x:c r="D11">
-        <x:v>102.992862138428</x:v>
+        <x:v>64.9294338491417</x:v>
       </x:c>
       <x:c r="E11">
-        <x:v>155.055406389318</x:v>
+        <x:v>169.169574309685</x:v>
       </x:c>
       <x:c r="F11">
-        <x:v>1.19372345562732</x:v>
+        <x:v>65.1612585713906</x:v>
       </x:c>
       <x:c r="G11">
-        <x:v>144.185319610026</x:v>
+        <x:v>86.0241528069713</x:v>
       </x:c>
       <x:c r="H11">
-        <x:v>180.206969464294</x:v>
+        <x:v>150.237977760955</x:v>
       </x:c>
       <x:c r="I11">
-        <x:v>40.4375253433536</x:v>
+        <x:v>38.3760117173083</x:v>
       </x:c>
       <x:c r="J11">
-        <x:v>66.2900019745762</x:v>
+        <x:v>75.4200443976652</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
       <x:c r="A12">
-        <x:v>89.6860760122939</x:v>
+        <x:v>2.53675123794784</x:v>
       </x:c>
       <x:c r="B12">
-        <x:v>118.527690003872</x:v>
+        <x:v>52.4431465437837</x:v>
       </x:c>
       <x:c r="C12">
-        <x:v>93.2372822860429</x:v>
+        <x:v>27.5361165532545</x:v>
       </x:c>
       <x:c r="D12">
-        <x:v>71.4456851926845</x:v>
+        <x:v>109.831803063784</x:v>
       </x:c>
       <x:c r="E12">
-        <x:v>173.181270329832</x:v>
+        <x:v>104.237139366678</x:v>
       </x:c>
       <x:c r="F12">
-        <x:v>111.72468890982</x:v>
+        <x:v>96.5307602177052</x:v>
       </x:c>
       <x:c r="G12">
-        <x:v>191.532829493067</x:v>
+        <x:v>47.6713096944947</x:v>
       </x:c>
       <x:c r="H12">
-        <x:v>80.1407568529904</x:v>
+        <x:v>136.000256676227</x:v>
       </x:c>
       <x:c r="I12">
-        <x:v>176.60873819916</x:v>
+        <x:v>139.157079597543</x:v>
       </x:c>
       <x:c r="J12">
-        <x:v>23.9589353203582</x:v>
+        <x:v>28.7473383493476</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
       <x:c r="A13">
-        <x:v>66.0129369543926</x:v>
+        <x:v>140.807224223766</x:v>
       </x:c>
       <x:c r="B13">
-        <x:v>1.17741571794144</x:v>
+        <x:v>52.7106113977314</x:v>
       </x:c>
       <x:c r="C13">
-        <x:v>186.733284213922</x:v>
+        <x:v>184.832931302876</x:v>
       </x:c>
       <x:c r="D13">
-        <x:v>127.14853581374</x:v>
+        <x:v>67.0119863315541</x:v>
       </x:c>
       <x:c r="E13">
-        <x:v>7.76534099493424</x:v>
+        <x:v>30.790216862592</x:v>
       </x:c>
       <x:c r="F13">
-        <x:v>80.7372552718675</x:v>
+        <x:v>176.609724842296</x:v>
       </x:c>
       <x:c r="G13">
-        <x:v>72.9986588810564</x:v>
+        <x:v>180.237860968447</x:v>
       </x:c>
       <x:c r="H13">
-        <x:v>163.782999182019</x:v>
+        <x:v>71.1506246920445</x:v>
       </x:c>
       <x:c r="I13">
-        <x:v>56.6358625221233</x:v>
+        <x:v>118.938880003495</x:v>
       </x:c>
       <x:c r="J13">
-        <x:v>109.665224100307</x:v>
+        <x:v>34.4971641127473</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
       <x:c r="A14">
-        <x:v>185.15272447148</x:v>
+        <x:v>117.622117101039</x:v>
       </x:c>
       <x:c r="B14">
-        <x:v>124.052693380067</x:v>
+        <x:v>110.893332357934</x:v>
       </x:c>
       <x:c r="C14">
-        <x:v>192.091737683905</x:v>
+        <x:v>79.9020451865634</x:v>
       </x:c>
       <x:c r="D14">
-        <x:v>146.017215748326</x:v>
+        <x:v>44.3261203562497</x:v>
       </x:c>
       <x:c r="E14">
-        <x:v>126.015437173664</x:v>
+        <x:v>161.165868472851</x:v>
       </x:c>
       <x:c r="F14">
-        <x:v>198.727653920058</x:v>
+        <x:v>10.9307847036658</x:v>
       </x:c>
       <x:c r="G14">
-        <x:v>96.5645972157664</x:v>
+        <x:v>106.114980069043</x:v>
       </x:c>
       <x:c r="H14">
-        <x:v>128.027825489653</x:v>
+        <x:v>149.464670172643</x:v>
       </x:c>
       <x:c r="I14">
-        <x:v>32.3683289030419</x:v>
+        <x:v>3.97442570141257</x:v>
       </x:c>
       <x:c r="J14">
-        <x:v>139.83291952863</x:v>
+        <x:v>76.8146358788082</x:v>
       </x:c>
     </x:row>
     <x:row r="15">
       <x:c r="A15">
-        <x:v>156.464440820955</x:v>
+        <x:v>44.2165598479177</x:v>
       </x:c>
       <x:c r="B15">
-        <x:v>197.059137465925</x:v>
+        <x:v>162.932115030909</x:v>
       </x:c>
       <x:c r="C15">
-        <x:v>135.062910027366</x:v>
+        <x:v>116.769280525283</x:v>
       </x:c>
       <x:c r="D15">
-        <x:v>102.8139430577</x:v>
+        <x:v>13.1734127240132</x:v>
       </x:c>
       <x:c r="E15">
-        <x:v>26.6380326015121</x:v>
+        <x:v>16.2347613909444</x:v>
       </x:c>
       <x:c r="F15">
-        <x:v>51.1551420442551</x:v>
+        <x:v>157.918465769812</x:v>
       </x:c>
       <x:c r="G15">
-        <x:v>77.7244538430704</x:v>
+        <x:v>24.8774865758035</x:v>
       </x:c>
       <x:c r="H15">
-        <x:v>176.988555945916</x:v>
+        <x:v>194.099975188309</x:v>
       </x:c>
       <x:c r="I15">
-        <x:v>2.17823824015364</x:v>
+        <x:v>14.9311195197194</x:v>
       </x:c>
       <x:c r="J15">
-        <x:v>28.1728979331315</x:v>
+        <x:v>179.578932365206</x:v>
       </x:c>
     </x:row>
     <x:row r="16">
       <x:c r="A16">
-        <x:v>128.70521532777</x:v>
+        <x:v>19.8511197324149</x:v>
       </x:c>
       <x:c r="B16">
-        <x:v>44.9744661548056</x:v>
+        <x:v>49.9856440583177</x:v>
       </x:c>
       <x:c r="C16">
-        <x:v>182.364267382009</x:v>
+        <x:v>141.767362943742</x:v>
       </x:c>
       <x:c r="D16">
-        <x:v>40.1767881774235</x:v>
+        <x:v>151.375606447168</x:v>
       </x:c>
       <x:c r="E16">
-        <x:v>76.825483085972</x:v>
+        <x:v>6.87868586130379</x:v>
       </x:c>
       <x:c r="F16">
-        <x:v>133.529605778646</x:v>
+        <x:v>144.807912663002</x:v>
       </x:c>
       <x:c r="G16">
-        <x:v>158.69570065229</x:v>
+        <x:v>54.6810515479562</x:v>
       </x:c>
       <x:c r="H16">
-        <x:v>115.527474188957</x:v>
+        <x:v>187.289033917379</x:v>
       </x:c>
       <x:c r="I16">
-        <x:v>95.227521143494</x:v>
+        <x:v>34.1392169865497</x:v>
       </x:c>
       <x:c r="J16">
-        <x:v>74.3181511174506</x:v>
+        <x:v>192.559849467389</x:v>
       </x:c>
     </x:row>
     <x:row r="17">
       <x:c r="A17">
-        <x:v>128.195064574571</x:v>
+        <x:v>84.9233976029434</x:v>
       </x:c>
       <x:c r="B17">
-        <x:v>180.402320428007</x:v>
+        <x:v>14.8735281149268</x:v>
       </x:c>
       <x:c r="C17">
-        <x:v>123.571106942171</x:v>
+        <x:v>31.2990977574601</x:v>
       </x:c>
       <x:c r="D17">
-        <x:v>130.772301243046</x:v>
+        <x:v>3.87884760456106</x:v>
       </x:c>
       <x:c r="E17">
-        <x:v>81.1372775030962</x:v>
+        <x:v>157.797927296626</x:v>
       </x:c>
       <x:c r="F17">
-        <x:v>165.633382632226</x:v>
+        <x:v>91.6434188800135</x:v>
       </x:c>
       <x:c r="G17">
-        <x:v>126.435952319967</x:v>
+        <x:v>172.54110135722</x:v>
       </x:c>
       <x:c r="H17">
-        <x:v>147.220066537717</x:v>
+        <x:v>183.209996197005</x:v>
       </x:c>
       <x:c r="I17">
-        <x:v>145.43024801902</x:v>
+        <x:v>148.665934590933</x:v>
       </x:c>
       <x:c r="J17">
-        <x:v>174.453616409774</x:v>
+        <x:v>93.3063546630118</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
       <x:c r="A18">
-        <x:v>15.1600916940533</x:v>
+        <x:v>190.415780148663</x:v>
       </x:c>
       <x:c r="B18">
-        <x:v>63.5050040034135</x:v>
+        <x:v>98.2066395218515</x:v>
       </x:c>
       <x:c r="C18">
-        <x:v>47.7724279499484</x:v>
+        <x:v>132.025830974814</x:v>
       </x:c>
       <x:c r="D18">
-        <x:v>36.7758186705298</x:v>
+        <x:v>62.3424437187344</x:v>
       </x:c>
       <x:c r="E18">
-        <x:v>67.4944944994033</x:v>
+        <x:v>184.53077850143</x:v>
       </x:c>
       <x:c r="F18">
-        <x:v>68.9537994884671</x:v>
+        <x:v>177.875109192857</x:v>
       </x:c>
       <x:c r="G18">
-        <x:v>66.1145056905758</x:v>
+        <x:v>135.941330872449</x:v>
       </x:c>
       <x:c r="H18">
-        <x:v>83.9193411562216</x:v>
+        <x:v>171.659518578863</x:v>
       </x:c>
       <x:c r="I18">
-        <x:v>100.510503212228</x:v>
+        <x:v>50.7772249406098</x:v>
       </x:c>
       <x:c r="J18">
-        <x:v>156.610198950679</x:v>
+        <x:v>72.8717510927803</x:v>
       </x:c>
     </x:row>
     <x:row r="19">
       <x:c r="A19">
-        <x:v>3.0128014287971</x:v>
+        <x:v>151.732238266492</x:v>
       </x:c>
       <x:c r="B19">
-        <x:v>96.0101029351401</x:v>
+        <x:v>186.137885780138</x:v>
       </x:c>
       <x:c r="C19">
-        <x:v>161.604760941865</x:v>
+        <x:v>56.2195051723251</x:v>
       </x:c>
       <x:c r="D19">
-        <x:v>28.4629645889918</x:v>
+        <x:v>139.359947638288</x:v>
       </x:c>
       <x:c r="E19">
-        <x:v>180.960008772537</x:v>
+        <x:v>14.6460443803324</x:v>
       </x:c>
       <x:c r="F19">
-        <x:v>140.178258316674</x:v>
+        <x:v>67.6364730427212</x:v>
       </x:c>
       <x:c r="G19">
-        <x:v>141.688425998058</x:v>
+        <x:v>169.125969414192</x:v>
       </x:c>
       <x:c r="H19">
-        <x:v>151.914949506482</x:v>
+        <x:v>128.526438739396</x:v>
       </x:c>
       <x:c r="I19">
-        <x:v>69.1917326623535</x:v>
+        <x:v>37.4474344949459</x:v>
       </x:c>
       <x:c r="J19">
-        <x:v>192.485831395018</x:v>
+        <x:v>16.3579558098493</x:v>
       </x:c>
     </x:row>
     <x:row r="20">
       <x:c r="A20">
-        <x:v>40.031953267768</x:v>
+        <x:v>156.24973315571</x:v>
       </x:c>
       <x:c r="B20">
-        <x:v>181.037123026809</x:v>
+        <x:v>118.825946151664</x:v>
       </x:c>
       <x:c r="C20">
-        <x:v>32.8003043461592</x:v>
+        <x:v>115.325453186094</x:v>
       </x:c>
       <x:c r="D20">
-        <x:v>158.050177785591</x:v>
+        <x:v>11.4145762340234</x:v>
       </x:c>
       <x:c r="E20">
-        <x:v>11.6378549540592</x:v>
+        <x:v>191.891238275865</x:v>
       </x:c>
       <x:c r="F20">
-        <x:v>176.062120392948</x:v>
+        <x:v>29.3430317329909</x:v>
       </x:c>
       <x:c r="G20">
-        <x:v>73.4880305237547</x:v>
+        <x:v>131.633017273449</x:v>
       </x:c>
       <x:c r="H20">
-        <x:v>4.29060878431919</x:v>
+        <x:v>112.890432920722</x:v>
       </x:c>
       <x:c r="I20">
-        <x:v>21.6766655546039</x:v>
+        <x:v>55.3754854273868</x:v>
       </x:c>
       <x:c r="J20">
-        <x:v>61.0046499692857</x:v>
+        <x:v>124.591342510931</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>